<commit_message>
Implemented no-argument constructor and getter/setter methods in PaymentRequestPayloadGeneratorGetterAndSetter class to pass values. Created custom constructors in PaymentRequestPayloadGeneratorByConstructor class to build payload. Demonstrated the benefits of using generators to create complex payloads by implementing Lombok Library Builders in PaymentRequestPayloadGeneratorByUsingBuilders class.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API_TestData.xlsx
+++ b/src/test/resources/TestData/API_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StreamPC\IdeaProjects\Dover\Dover_Assesment\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1AEA1E-DFE8-4FA5-8D6A-1C2CDEEAB9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC747DAE-665F-4438-9049-C63C64C04214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment1" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="193">
   <si>
     <t>Street</t>
   </si>
@@ -590,15 +590,12 @@
     <t>TEB</t>
   </si>
   <si>
-    <t>pymtinf.amt.ccy</t>
+    <t>pymtinf.amt</t>
   </si>
   <si>
     <t xml:space="preserve"> Status</t>
   </si>
   <si>
-    <t>pymtinf.amt.amt</t>
-  </si>
-  <si>
     <t>10000</t>
   </si>
   <si>
@@ -615,6 +612,9 @@
   </si>
   <si>
     <t>KRASDFAS</t>
+  </si>
+  <si>
+    <t>pymtinf.ccy</t>
   </si>
   <si>
     <t>paymentStatus</t>
@@ -1149,10 +1149,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2502,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F052F1CC-3304-48FC-A88A-CE0AB45A4F1D}">
-  <dimension ref="A1:AC15"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,7 +2540,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2601,10 +2601,10 @@
       <c r="O2" s="45"/>
       <c r="P2" s="45"/>
       <c r="Q2" s="46"/>
-      <c r="R2" s="71" t="s">
+      <c r="R2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="72"/>
+      <c r="S2" s="71"/>
       <c r="T2" s="63"/>
       <c r="U2" s="54" t="s">
         <v>184</v>
@@ -2648,10 +2648,8 @@
         <v>107</v>
       </c>
       <c r="Q3" s="41"/>
-      <c r="R3" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="S3" s="49"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="72"/>
       <c r="T3" s="63"/>
       <c r="U3" s="55"/>
       <c r="V3" s="38" t="s">
@@ -2767,7 +2765,7 @@
         <v>111</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>112</v>
@@ -2779,10 +2777,10 @@
         <v>114</v>
       </c>
       <c r="R5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="S5" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="T5" s="67" t="s">
         <v>177</v>
@@ -2822,7 +2820,7 @@
         <v>TC_1_IP_From_TR_To_US</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" t="s">
         <v>135</v>
@@ -2855,7 +2853,7 @@
         <v>149</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T6">
         <v>202</v>
@@ -3027,7 +3025,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="7" t="str">
@@ -3041,7 +3039,7 @@
         <v>134</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="0"/>
@@ -3071,28 +3069,16 @@
         <v>|TC_5_IP_From_TR_To_US||</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:29" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G15" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="AC1:AC4"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R3:S3"/>
     <mergeCell ref="U1:Z1"/>
     <mergeCell ref="U2:U4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="T1:T4"/>
+    <mergeCell ref="R2:S3"/>
     <mergeCell ref="E1:S1"/>
     <mergeCell ref="V2:Z2"/>
     <mergeCell ref="V3:V4"/>

</xml_diff>

<commit_message>
Setting up the framework to Mac
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/API_TestData.xlsx
+++ b/src/test/resources/TestData/API_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StreamPC\IdeaProjects\Dover\Dover_Assesment\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hamza/IdeaProjects/smartbearsoftware/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E15F5F7-1119-40DC-9C6F-3903A0417BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DFC270-A38E-DC43-8912-9565A5E0A8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-2460" windowWidth="51200" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payment1" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="194">
   <si>
     <t>Street</t>
   </si>
@@ -618,6 +617,9 @@
   </si>
   <si>
     <t>paymentStatus</t>
+  </si>
+  <si>
+    <t>cdtr.bank.bicNb</t>
   </si>
 </sst>
 </file>
@@ -969,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -992,167 +994,165 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1444,83 +1444,83 @@
       <selection pane="bottomRight" activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="18" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="18" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:24" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="26"/>
-      <c r="X1" s="21" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
+      <c r="X1" s="25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+    <row r="2" spans="1:24" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="18" t="s">
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="18" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="19"/>
-      <c r="U2" s="20"/>
-      <c r="X2" s="22"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="24"/>
+      <c r="X2" s="26"/>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1585,20 +1585,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="27" t="s">
         <v>75</v>
       </c>
       <c r="F4" s="7" t="str">
@@ -1655,16 +1655,16 @@
         <v>|TC_1_Test|</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="7" t="str">
         <f>_xlfn.CONCAT("TC_",A5,"_",B5)</f>
         <v>TC_2_Yeni_Istanbul</v>
@@ -1719,16 +1719,16 @@
         <v>|TC_2_Yeni_Istanbul|</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="7" t="str">
         <f>_xlfn.CONCAT("TC_",A6,"_",B6)</f>
         <v>TC_3_Yeni_Ankara</v>
@@ -1783,16 +1783,16 @@
         <v>|TC_3_Yeni_Ankara|</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
       <c r="F7" s="7" t="str">
         <f t="shared" ref="F7:F10" si="0">_xlfn.CONCAT("TC_",A7,"_",B7)</f>
         <v>TC_4_Test Info</v>
@@ -1847,16 +1847,16 @@
         <v>|TC_4_Test Info|</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>TC_5_Order_EG_Egypt_Client</v>
@@ -1909,16 +1909,16 @@
         <v>|TC_5_Order_EG_Egypt_Client|</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="7" t="str">
         <f>_xlfn.CONCAT("TC_",A9,"_",B9)</f>
         <v>TC_6_Order_KR_ SouthKorea_Client</v>
@@ -1973,16 +1973,16 @@
         <v>|TC_6_Order_KR_ SouthKorea_Client|</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>TC_7_Order_TR_Turkiye_Client</v>
@@ -2037,20 +2037,20 @@
         <v>|TC_7_Order_TR_Turkiye_Client|</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F11" s="10" t="str">
@@ -2107,16 +2107,16 @@
         <v>|TC_1_Order_Wrong_Product_Name|</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="9" t="str">
         <f>_xlfn.CONCAT("TC_",A12,"_",B12)</f>
         <v>TC_1_Order_Empty_Customer_Name</v>
@@ -2169,16 +2169,16 @@
         <v>|TC_1_Order_Empty_Customer_Name|</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="9" t="str">
         <f>_xlfn.CONCAT("TC_",A13,"_",B13)</f>
         <v>TC_1_Order_Empty_Street</v>
@@ -2231,16 +2231,16 @@
         <v>|TC_1_Order_Empty_Street|</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="9" t="str">
         <f>_xlfn.CONCAT("TC_",A14,"_",B14)</f>
         <v>TC_1_Order_Empty_City</v>
@@ -2293,16 +2293,16 @@
         <v>|TC_1_Order_Empty_City|</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="9" t="str">
         <f>_xlfn.CONCAT("TC_",A15,"_",B15)</f>
         <v>TC_1_Order_Empty_Zip</v>
@@ -2355,16 +2355,16 @@
         <v>|TC_1_Order_Empty_Zip|</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="9" t="str">
         <f t="shared" ref="F16:F17" si="2">_xlfn.CONCAT("TC_",A16,"_",B16)</f>
         <v>TC_1_Order_Empty_Card_Number</v>
@@ -2417,16 +2417,16 @@
         <v>|TC_1_Order_Empty_Card_Number|</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="9" t="str">
         <f t="shared" si="2"/>
         <v>TC_1_Order_Empty_Expire_Date</v>
@@ -2481,6 +2481,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D4:D10"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="C11:C17"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="E4:E10"/>
@@ -2488,11 +2493,6 @@
     <mergeCell ref="I1:U1"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="I2:M2"/>
-    <mergeCell ref="D4:D10"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="C11:C17"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2504,227 +2504,227 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F052F1CC-3304-48FC-A88A-CE0AB45A4F1D}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" activeCellId="1" sqref="I14 I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="53.28515625" customWidth="1"/>
+    <col min="24" max="24" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="50" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="62" t="s">
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AC1" s="68" t="s">
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AC1" s="38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="38" t="s">
+    <row r="2" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44" t="s">
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="32" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="71"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="54" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="V2" s="44" t="s">
+      <c r="V2" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="46"/>
-      <c r="AC2" s="69"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="49"/>
+      <c r="AC2" s="39"/>
     </row>
-    <row r="3" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="38" t="s">
+    <row r="3" spans="1:29" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="40" t="s">
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="61"/>
+      <c r="L3" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="40" t="s">
+      <c r="N3" s="60"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="72"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="38" t="s">
+      <c r="Q3" s="61"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="W3" s="40" t="s">
+      <c r="W3" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="41"/>
-      <c r="AC3" s="69"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="61"/>
+      <c r="AC3" s="39"/>
     </row>
-    <row r="4" spans="1:29" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="42" t="s">
+    <row r="4" spans="1:29" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="42" t="s">
+      <c r="L4" s="46"/>
+      <c r="M4" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="N4" s="42" t="s">
+      <c r="N4" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="O4" s="43" t="s">
+      <c r="O4" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="Q4" s="43" t="s">
+      <c r="Q4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="R4" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="S4" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="T4" s="64"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="61" t="s">
+      <c r="T4" s="53"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="X4" s="43" t="s">
+      <c r="X4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="Y4" s="43" t="s">
+      <c r="Y4" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="Z4" s="43" t="s">
+      <c r="Z4" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="AC4" s="69"/>
+      <c r="AC4" s="39"/>
     </row>
-    <row r="5" spans="1:29" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>111</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>188</v>
@@ -2782,7 +2782,7 @@
       <c r="S5" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="T5" s="67" t="s">
+      <c r="T5" s="21" t="s">
         <v>177</v>
       </c>
       <c r="U5" s="6" t="s">
@@ -2805,21 +2805,21 @@
       </c>
       <c r="AC5"/>
     </row>
-    <row r="6" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="27" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="7" t="str">
         <f>_xlfn.CONCAT("TC_",A6,"_",B6)</f>
         <v>TC_1_IP_From_TR_To_US</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="20" t="s">
         <v>187</v>
       </c>
       <c r="F6" t="s">
@@ -2831,7 +2831,7 @@
       <c r="I6" t="s">
         <v>182</v>
       </c>
-      <c r="J6" s="70" t="s">
+      <c r="J6" t="s">
         <v>178</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -2881,19 +2881,19 @@
         <v>|TC_1_IP_From_TR_To_US|202|</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="7" t="str">
         <f t="shared" ref="D7:D10" si="1">_xlfn.CONCAT("TC_",A7,"_",B7)</f>
         <v>TC_2_IP_From_BE_To_ES</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="20" t="s">
         <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -2917,7 +2917,7 @@
       <c r="O7" t="s">
         <v>147</v>
       </c>
-      <c r="P7" s="58" t="s">
+      <c r="P7" s="18" t="s">
         <v>145</v>
       </c>
       <c r="R7" t="s">
@@ -2952,19 +2952,19 @@
         <v>|TC_2_IP_From_BE_To_ES|202|</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>161</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>TC_3_IP_From_DE_To_UK</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="20" t="s">
         <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -3020,22 +3020,22 @@
         <v>|TC_3_IP_From_DE_To_UK|202|</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="7" t="str">
         <f>_xlfn.CONCAT("TC_",A9,"_",B9)</f>
         <v>TC_4_IP_From_KR_To_US</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G9" t="s">
@@ -3046,22 +3046,22 @@
         <v>|TC_4_IP_From_KR_To_US||</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>TC_5_IP_From_TR_To_US</v>
       </c>
-      <c r="E10" s="65" t="s">
+      <c r="E10" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="2" t="s">
         <v>135</v>
       </c>
       <c r="AC10" t="str">
@@ -3071,18 +3071,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AC1:AC4"/>
-    <mergeCell ref="U1:Z1"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="T1:T4"/>
-    <mergeCell ref="R2:S3"/>
-    <mergeCell ref="E1:S1"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:Z3"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J3:K3"/>
@@ -3091,6 +3079,18 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="T1:T4"/>
+    <mergeCell ref="R2:S3"/>
+    <mergeCell ref="E1:S1"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="AC1:AC4"/>
+    <mergeCell ref="U1:Z1"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F2:K2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3104,7 +3104,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>